<commit_message>
feat: İskonto girişi ve DB'ye kaydetme özelliği eklendi
- Modal'e iskonto (%) girişi eklendi
- İki buton: Sadece Şimdi Kullan ve Kaydet ve Kullan
- Backend'e add-option endpoint'i eklendi
- Yeni/mevcut option'lar DB'ye kaydedilebiliyor
- Option güncellemesi dropdown'u otomatik yeniliyor
- Portal uyumluluğu korundu
</commit_message>
<xml_diff>
--- a/fiyat_tablosu_3.xlsx
+++ b/fiyat_tablosu_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mira\hidrolik-silindir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DF04028F-E0FE-458A-A0EE-36E061AA904D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BD998B-674C-4518-9A25-B994D16E6D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boru" sheetId="1" r:id="rId1"/>
@@ -277,7 +277,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -286,13 +286,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -310,7 +325,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -325,7 +340,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -334,13 +349,11 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -349,13 +362,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -364,11 +377,84 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -383,6 +469,19 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -398,106 +497,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -507,87 +507,53 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -601,6 +567,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -884,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E27"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,237 +871,237 @@
     <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="27" t="s">
+    <row r="1" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="32" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="16">
         <v>29.33</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="6">
         <v>50</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="16">
         <v>35.28</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>50</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="16">
         <v>53.08</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>50</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="16">
         <v>76.930000000000007</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>60</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="16">
         <v>94.35</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>60</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="16">
         <v>158.94999999999999</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>70</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="16">
         <v>176.8</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>70</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="16">
         <v>206</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>80</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="16">
         <v>391</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>80</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="16">
         <v>473.25</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>100</v>
       </c>
-      <c r="E11" s="21">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="1" t="s">
+      <c r="E11" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="16">
         <v>817.7</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>100</v>
       </c>
-      <c r="E12" s="23">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="3" t="s">
+      <c r="E12" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="16">
         <v>918</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>120</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="17">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C16" s="5"/>
-      <c r="E16" s="33"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17" s="5"/>
-      <c r="E17" s="33"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C18" s="5"/>
-      <c r="E18" s="33"/>
+      <c r="E18" s="29"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C19" s="5"/>
-      <c r="E19" s="33"/>
+      <c r="E19" s="29"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C20" s="5"/>
-      <c r="E20" s="33"/>
+      <c r="E20" s="29"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C21" s="5"/>
-      <c r="E21" s="33"/>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C22" s="5"/>
-      <c r="E22" s="33"/>
+      <c r="E22" s="29"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C23" s="5"/>
-      <c r="E23" s="33"/>
+      <c r="E23" s="29"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C24" s="5"/>
-      <c r="E24" s="33"/>
+      <c r="E24" s="29"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C25" s="5"/>
-      <c r="E25" s="33"/>
+      <c r="E25" s="29"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C26" s="5"/>
-      <c r="E26" s="33"/>
+      <c r="E26" s="29"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.35">
       <c r="D27" s="5"/>
@@ -1142,20 +1117,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E24C85-5058-49AD-B39A-ED0D5BFF462B}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="W41" sqref="W41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1166,7 +1141,7 @@
       <c r="B2" s="2">
         <v>7</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1177,7 +1152,7 @@
       <c r="B3" s="2">
         <v>7</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1188,7 +1163,7 @@
       <c r="B4" s="2">
         <v>9</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1199,7 +1174,7 @@
       <c r="B5" s="2">
         <v>10</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1210,7 +1185,7 @@
       <c r="B6" s="2">
         <v>11</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1221,7 +1196,7 @@
       <c r="B7" s="2">
         <v>17</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1232,7 +1207,7 @@
       <c r="B8" s="2">
         <v>20</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1243,7 +1218,7 @@
       <c r="B9" s="2">
         <v>25</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1254,7 +1229,7 @@
       <c r="B10" s="2">
         <v>45</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1265,7 +1240,7 @@
       <c r="B11" s="2">
         <v>50</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1276,7 +1251,7 @@
       <c r="B12" s="4">
         <v>75</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1302,13 +1277,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1316,10 +1291,10 @@
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="16">
         <v>3.39</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1327,10 +1302,10 @@
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1338,10 +1313,10 @@
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="16">
         <v>5.64</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1349,10 +1324,10 @@
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <v>8.81</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1360,10 +1335,10 @@
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <v>12.39</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1371,10 +1346,10 @@
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="16">
         <v>20.64</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1382,10 +1357,10 @@
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <v>24.96</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1393,10 +1368,10 @@
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="16">
         <v>31.44</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1404,10 +1379,10 @@
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="16">
         <v>54.33</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1415,10 +1390,10 @@
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="16">
         <v>68</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1426,10 +1401,10 @@
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="16">
         <v>82</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1437,101 +1412,101 @@
       <c r="A13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>95</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
-      <c r="C16" s="33"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
-      <c r="C17" s="33"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="33"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
-      <c r="C19" s="33"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="33"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
-      <c r="C21" s="33"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
-      <c r="C24" s="33"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
-      <c r="C25" s="33"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
-      <c r="C26" s="33"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
-      <c r="C27" s="33"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
-      <c r="C28" s="33"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
-      <c r="C29" s="33"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
-      <c r="C31" s="33"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
-      <c r="C32" s="33"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
-      <c r="C33" s="33"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
-      <c r="C34" s="33"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
-      <c r="C35" s="33"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="5"/>
-      <c r="C36" s="33"/>
+      <c r="C36" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1555,13 +1530,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1569,10 +1544,10 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="16">
         <v>2.58</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1580,10 +1555,10 @@
       <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <v>3.05</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1591,10 +1566,10 @@
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="16">
         <v>4.2300000000000004</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1602,10 +1577,10 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <v>1.23</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1613,10 +1588,10 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <v>7.38</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1624,10 +1599,10 @@
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="16">
         <v>10.84</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1635,10 +1610,10 @@
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <v>17.46</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1646,10 +1621,10 @@
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="16">
         <v>24.95</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1657,10 +1632,10 @@
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="16">
         <v>32.89</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1668,10 +1643,10 @@
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="16">
         <v>61.95</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>25</v>
       </c>
     </row>
@@ -1679,61 +1654,61 @@
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>102.9</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
-      <c r="C16" s="33"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
-      <c r="C17" s="33"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="33"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
-      <c r="C19" s="33"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="33"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
-      <c r="C21" s="33"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
-      <c r="C24" s="33"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
-      <c r="C25" s="33"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
-      <c r="C26" s="33"/>
+      <c r="C26" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1757,13 +1732,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1774,7 +1749,7 @@
       <c r="B2" s="2">
         <v>5</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1785,7 +1760,7 @@
       <c r="B3" s="2">
         <v>6</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1796,7 +1771,7 @@
       <c r="B4" s="2">
         <v>8</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1807,7 +1782,7 @@
       <c r="B5" s="2">
         <v>12</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1818,7 +1793,7 @@
       <c r="B6" s="2">
         <v>13</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1829,7 +1804,7 @@
       <c r="B7" s="2">
         <v>14</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1840,7 +1815,7 @@
       <c r="B8" s="2">
         <v>28</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1851,7 +1826,7 @@
       <c r="B9" s="2">
         <v>33</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1862,7 +1837,7 @@
       <c r="B10" s="2">
         <v>56</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1873,7 +1848,7 @@
       <c r="B11" s="2">
         <v>58</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1884,85 +1859,85 @@
       <c r="B12" s="2">
         <v>62</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C16" s="33"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C17" s="33"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C18" s="33"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C19" s="33"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C20" s="33"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C21" s="33"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C22" s="33"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C23" s="33"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C24" s="33"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
-      <c r="C25" s="33"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
-      <c r="C26" s="33"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" s="5"/>
-      <c r="C27" s="33"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" s="5"/>
-      <c r="C28" s="33"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" s="5"/>
-      <c r="C29" s="33"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" s="5"/>
-      <c r="C30" s="33"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" s="5"/>
-      <c r="C31" s="33"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
-      <c r="C32" s="33"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="5"/>
-      <c r="C33" s="33"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="5"/>
-      <c r="C34" s="33"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="5"/>
-      <c r="C35" s="33"/>
+      <c r="C35" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1985,13 +1960,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2002,7 +1977,7 @@
       <c r="B2" s="2">
         <v>20</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2013,7 +1988,7 @@
       <c r="B3" s="2">
         <v>20</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2024,7 +1999,7 @@
       <c r="B4" s="2">
         <v>25</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2035,7 +2010,7 @@
       <c r="B5" s="2">
         <v>30</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2046,7 +2021,7 @@
       <c r="B6" s="2">
         <v>45</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2057,7 +2032,7 @@
       <c r="B7" s="2">
         <v>150</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2068,7 +2043,7 @@
       <c r="B8" s="2">
         <v>200</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2079,7 +2054,7 @@
       <c r="B9" s="2">
         <v>250</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2090,7 +2065,7 @@
       <c r="B10" s="2">
         <v>400</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2101,7 +2076,7 @@
       <c r="B11" s="2">
         <v>430</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2112,58 +2087,58 @@
       <c r="B12" s="4">
         <v>470</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="32"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
-      <c r="C16" s="33"/>
+      <c r="C16" s="29"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
-      <c r="C17" s="33"/>
+      <c r="C17" s="29"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="33"/>
+      <c r="C18" s="29"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="5"/>
-      <c r="C19" s="33"/>
+      <c r="C19" s="29"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="5"/>
-      <c r="C20" s="33"/>
+      <c r="C20" s="29"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="5"/>
-      <c r="C21" s="33"/>
+      <c r="C21" s="29"/>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="5"/>
-      <c r="C22" s="33"/>
+      <c r="C22" s="29"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="5"/>
-      <c r="C23" s="33"/>
+      <c r="C23" s="29"/>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="5"/>
-      <c r="C24" s="33"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25" s="5"/>
-      <c r="C25" s="33"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26" s="5"/>
-      <c r="C26" s="33"/>
+      <c r="C26" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2186,16 +2161,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2209,7 +2184,7 @@
       <c r="C2" s="7">
         <v>160</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2223,7 +2198,7 @@
       <c r="C3" s="8">
         <v>160</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2237,7 +2212,7 @@
       <c r="C4" s="8">
         <v>160</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2251,7 +2226,7 @@
       <c r="C5" s="8">
         <v>170</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2265,7 +2240,7 @@
       <c r="C6" s="8">
         <v>170</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2279,7 +2254,7 @@
       <c r="C7" s="8">
         <v>200</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2293,7 +2268,7 @@
       <c r="C8" s="8">
         <v>200</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2307,7 +2282,7 @@
       <c r="C9" s="8">
         <v>200</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2321,7 +2296,7 @@
       <c r="C10" s="8">
         <v>230</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2335,7 +2310,7 @@
       <c r="C11" s="8">
         <v>230</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="18">
         <v>25</v>
       </c>
     </row>
@@ -2349,7 +2324,7 @@
       <c r="C12" s="9">
         <v>250</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="20">
         <v>25</v>
       </c>
     </row>
@@ -2366,23 +2341,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98098A22-921C-40A3-89A5-5CDFF78609F6}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2390,10 +2366,10 @@
       <c r="A2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="16">
         <v>8.69</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2401,10 +2377,10 @@
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="16">
         <v>10.050000000000001</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2412,10 +2388,10 @@
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="16">
         <v>11.59</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2423,10 +2399,10 @@
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="16">
         <v>17.39</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2434,10 +2410,10 @@
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="16">
         <v>21.25</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2445,10 +2421,10 @@
       <c r="A7" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="16">
         <v>74</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2456,10 +2432,10 @@
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="16">
         <v>40.57</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2467,10 +2443,10 @@
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="16">
         <v>63.76</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2478,8 +2454,8 @@
       <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2487,8 +2463,8 @@
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17">
         <v>25</v>
       </c>
     </row>
@@ -2496,71 +2472,71 @@
       <c r="A12" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2582,13 +2558,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2599,7 +2575,7 @@
       <c r="B2" s="2">
         <v>12</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2610,7 +2586,7 @@
       <c r="B3" s="2">
         <v>13</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2621,7 +2597,7 @@
       <c r="B4" s="2">
         <v>15</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2632,7 +2608,7 @@
       <c r="B5" s="2">
         <v>18</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2643,7 +2619,7 @@
       <c r="B6" s="2">
         <v>22</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2654,7 +2630,7 @@
       <c r="B7" s="2">
         <v>25</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2665,7 +2641,7 @@
       <c r="B8" s="2">
         <v>50</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2676,7 +2652,7 @@
       <c r="B9" s="2">
         <v>75</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2687,7 +2663,7 @@
       <c r="B10" s="2">
         <v>228</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2698,7 +2674,7 @@
       <c r="B11" s="2">
         <v>254</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2709,7 +2685,7 @@
       <c r="B12" s="4">
         <v>241</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>0</v>
       </c>
     </row>
@@ -2734,13 +2710,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2748,10 +2724,10 @@
       <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="21">
         <v>8.69</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2759,10 +2735,10 @@
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="24">
+      <c r="B3" s="21">
         <v>10.050000000000001</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2770,10 +2746,10 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="21">
         <v>11.59</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2781,10 +2757,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="21">
         <v>17.39</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2792,10 +2768,10 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="21">
         <v>21.25</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2803,10 +2779,10 @@
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="21">
         <v>40.57</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2814,10 +2790,10 @@
       <c r="A8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="21">
         <v>63.76</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2825,10 +2801,10 @@
       <c r="A9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="21">
         <v>139</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2836,10 +2812,10 @@
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="21">
         <v>85.01</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2847,10 +2823,10 @@
       <c r="A11" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="22">
         <v>271</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2858,10 +2834,10 @@
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="22">
         <v>385</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="20">
         <v>0</v>
       </c>
     </row>
@@ -2869,10 +2845,10 @@
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="22">
         <v>549</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2880,10 +2856,10 @@
       <c r="A14" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>783</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2891,10 +2867,10 @@
       <c r="A15" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="22">
         <v>798</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2902,10 +2878,10 @@
       <c r="A16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="25">
+      <c r="B16" s="22">
         <v>935</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2913,10 +2889,10 @@
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="25">
+      <c r="B17" s="22">
         <v>947</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2924,8 +2900,8 @@
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="21">
+      <c r="B18" s="22"/>
+      <c r="C18" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2933,8 +2909,8 @@
       <c r="A19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="21">
+      <c r="B19" s="22"/>
+      <c r="C19" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2942,8 +2918,8 @@
       <c r="A20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="21">
+      <c r="B20" s="22"/>
+      <c r="C20" s="18">
         <v>0</v>
       </c>
     </row>
@@ -2951,10 +2927,10 @@
       <c r="A21" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="22">
         <v>2000</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="18">
         <v>0</v>
       </c>
     </row>

</xml_diff>